<commit_message>
Disabled combinations that are difficult to see
</commit_message>
<xml_diff>
--- a/hack_graphics/hack_constraints.xlsx
+++ b/hack_graphics/hack_constraints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nas0\skynet\sboxes_gecko\sb0_gecko\hack_graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA8822D-10C3-4301-B79E-B76640ED9242}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5599BEF-801F-4930-9E4C-0BA1FBF10A17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="27">
   <si>
     <t>Circuit sclera_00000.jpg</t>
   </si>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,9 +562,7 @@
       <c r="O2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
         <v>26</v>
       </c>
@@ -615,9 +613,7 @@
       <c r="O3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
         <v>26</v>
       </c>
@@ -668,9 +664,7 @@
       <c r="O4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
         <v>26</v>
       </c>
@@ -721,9 +715,7 @@
       <c r="O5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" s="2" t="s">
         <v>26</v>
       </c>
@@ -774,9 +766,7 @@
       <c r="O6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P6" s="2"/>
       <c r="Q6" s="2" t="s">
         <v>26</v>
       </c>
@@ -827,12 +817,8 @@
       <c r="O7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -880,9 +866,7 @@
       <c r="O8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P8" s="2"/>
       <c r="Q8" s="2" t="s">
         <v>26</v>
       </c>
@@ -933,9 +917,7 @@
       <c r="O9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
         <v>26</v>
       </c>
@@ -986,9 +968,7 @@
       <c r="O10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
         <v>26</v>
       </c>

</xml_diff>